<commit_message>
update to mcode to 0.9.1 (fhir dstu 2)
</commit_message>
<xml_diff>
--- a/docs/mcode/onco-core-EvidenceType-extension.xlsx
+++ b/docs/mcode/onco-core-EvidenceType-extension.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="65">
   <si>
     <t>Path</t>
   </si>
@@ -137,23 +137,23 @@
     <t>EvidenceType</t>
   </si>
   <si>
-    <t>The type of evidence considered in making the determination.</t>
+    <t>Categorization of the kind of evidence used as input to the clinical judgment. This corresponds to both the S and O in SOAP.</t>
+  </si>
+  <si>
+    <t>Extension.id</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Extension.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t xml:space="preserve">id
 </t>
   </si>
   <si>
     <t>xml:id (or equivalent in JSON)</t>
   </si>
   <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>unique id for the element within a resource (for internal references).</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -162,11 +162,21 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>An Extension</t>
+    <t>Additional Content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
     <t>Element.extension</t>
@@ -175,7 +185,7 @@
     <t>Extension.url</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -185,13 +195,16 @@
     <t>Source of the definition for the extension code - a logical name or a URL.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://hl7.org/fhir/us/shr/StructureDefinition/onco-core-EvidenceType-extension"/&gt;</t>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition should be version specific.  This will ideally be the URI for the Resource Profile defining the extension, with the code for the extension after a #.</t>
+  </si>
+  <si>
+    <t>http://mcodeinitiative.org/us/mcode/StructureDefinition/onco-core-EvidenceType-extension</t>
   </si>
   <si>
     <t>Extension.valueCodeableConcept</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept {[]} {[]}
+    <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
@@ -254,67 +267,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -350,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -361,7 +374,7 @@
   <cols>
     <col min="1" max="1" width="30.890625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
@@ -369,7 +382,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.0859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="43.6640625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -591,7 +604,7 @@
         <v>37</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH2" t="s" s="2">
         <v>36</v>
@@ -602,7 +615,7 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -613,7 +626,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>36</v>
@@ -688,7 +701,7 @@
         <v>37</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>36</v>
@@ -703,7 +716,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
@@ -722,15 +735,17 @@
         <v>36</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="M4" t="s" s="2">
+        <v>52</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>36</v>
@@ -779,7 +794,7 @@
         <v>36</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>37</v>
@@ -796,7 +811,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -804,10 +819,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>36</v>
@@ -819,22 +834,24 @@
         <v>36</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="M5" t="s" s="2">
+        <v>58</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>36</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>36</v>
@@ -876,13 +893,13 @@
         <v>36</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>36</v>
@@ -893,7 +910,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -901,10 +918,10 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>36</v>
@@ -916,13 +933,13 @@
         <v>36</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -973,13 +990,13 @@
         <v>36</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>36</v>

</xml_diff>